<commit_message>
update task 4 data
</commit_message>
<xml_diff>
--- a/task_4_idef0/task_4_data.xlsx
+++ b/task_4_idef0/task_4_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleks\Documents\UrkSURT\Teaching\Інформаційні системи та технології\практичні роботи\task_3_kanban\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleks\Documents\UrkSURT\Teaching\Інформаційні системи і технології\практичні роботи\task_4_idef0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB32AE50-6BB8-4187-A456-4432C14BC64C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2C46F0C-95A5-4EAC-9C81-DAD18F017564}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
   <si>
     <t>Варіант</t>
   </si>
@@ -225,99 +225,6 @@
   </si>
   <si>
     <t>Впровадження розумних технологій для покращення міської інфраструктури та послуг.</t>
-  </si>
-  <si>
-    <t>Епік (приклад): Система аутентифікації користувачів. Завдання (приклад): Розробити схему бази даних для аутентифікації користувачів. Завдання (приклад): Реалізувати функціонал входу.</t>
-  </si>
-  <si>
-    <t>Епік (приклад): Логістика конференції. Завдання (приклад): Забронювати місце для конференції. Завдання (приклад): Організувати кейтеринг.</t>
-  </si>
-  <si>
-    <t>Епік (приклад): Огляд літератури. Завдання (приклад): Зібрати відповідні наукові статті. Завдання (приклад): Узагальнити основні висновки з літератури.</t>
-  </si>
-  <si>
-    <t>Епік (приклад): Кампанія в соціальних мережах. Завдання (приклад): Розробити рекламу для соціальних мереж. Завдання (приклад): Запланувати публікації в соціальних мережах.</t>
-  </si>
-  <si>
-    <t>Епік (приклад): Редизайн головної сторінки. Завдання (приклад): Створити вайрфрейми для нової головної сторінки. Завдання (приклад): Розробити макет головної сторінки в HTML/CSS.</t>
-  </si>
-  <si>
-    <t>Епік (приклад): Дослідження ринку. Завдання (приклад): Провести аналіз конкурентів. Завдання (приклад): Визначити цільову аудиторію.</t>
-  </si>
-  <si>
-    <t>Епік (приклад): Інтеграція платежів. Завдання (приклад): Інтегрувати платіжний шлюз. Завдання (приклад): Перевірити процес оплати різними методами.</t>
-  </si>
-  <si>
-    <t>Епік (приклад): Дизайн користувацького інтерфейсу. Завдання (приклад): Розробити прототип додатку. Завдання (приклад): Провести тестування зручності використання.</t>
-  </si>
-  <si>
-    <t>Епік (приклад): Міграція до хмари. Завдання (приклад): Мігрувати дані на хмарну платформу. Завдання (приклад): Навчити співробітників використанню нових хмарних інструментів.</t>
-  </si>
-  <si>
-    <t>Епік (приклад): Серія блогів. Завдання (приклад): Написати пост у блозі про галузеві тенденції. Завдання (приклад): Редагувати та публікувати пост у блозі.</t>
-  </si>
-  <si>
-    <t>Епік (приклад): Процес найму. Завдання (приклад): Створити вакансію для розробника програмного забезпечення. Завдання (приклад): Провести початкові співбесіди з кандидатами.</t>
-  </si>
-  <si>
-    <t>Епік (приклад): Підготовка внутрішнього аудиту. Завдання (приклад): Переглянути фінансові звіти компанії. Завдання (приклад): Підготувати аудиторську документацію.</t>
-  </si>
-  <si>
-    <t>Епік (приклад): Система підтримки заявок. Завдання (приклад): Розробити розділ FAQ для вебсайту. Завдання (приклад): Впровадити систему відстеження заявок.</t>
-  </si>
-  <si>
-    <t>Епік (приклад): Оцінка постачальників. Завдання (приклад): Оцінити продуктивність постачальників. Завдання (приклад): Переговорити умови контракту з постачальниками.</t>
-  </si>
-  <si>
-    <t>Епік (приклад): Розробка курсу. Завдання (приклад): Створити план курсу. Завдання (приклад): Розробити навчальні матеріали.</t>
-  </si>
-  <si>
-    <t>Епік (приклад): Система управління пацієнтами. Завдання (приклад): Розробити форму для прийому пацієнтів. Завдання (приклад): Впровадити систему електронних медичних записів.</t>
-  </si>
-  <si>
-    <t>Епік (приклад): Благодійний захід. Завдання (приклад): Спланувати логістику благодійного заходу. Завдання (приклад): Просувати захід у соціальних мережах.</t>
-  </si>
-  <si>
-    <t>Епік (приклад): Будівельні дозволи. Завдання (приклад): Отримати будівельні дозволи. Завдання (приклад): Координувати дії з місцевими органами влади.</t>
-  </si>
-  <si>
-    <t>Епік (приклад): Дизайн ідентичності бренду. Завдання (приклад): Розробити логотип для клієнта. Завдання (приклад): Створити гайдбук для бренду.</t>
-  </si>
-  <si>
-    <t>Епік (приклад): Кампанія з посадки дерев. Завдання (приклад): Організувати захід з посадки дерев. Завдання (приклад): Набрати волонтерів для кампанії.</t>
-  </si>
-  <si>
-    <t>Епік (приклад): Очищення даних. Завдання (приклад): Очистити та підготувати набір даних. Завдання (приклад): Провести розвідувальний аналіз даних.</t>
-  </si>
-  <si>
-    <t>Епік (приклад): Документація справи. Завдання (приклад): Підготувати юридичні документи для подання. Завдання (приклад): Переглянути докази по справі.</t>
-  </si>
-  <si>
-    <t>Епік (приклад): Управління інвентарем. Завдання (приклад): Провести інвентаризацію. Завдання (приклад): Перезамовити товари з низьким залишком.</t>
-  </si>
-  <si>
-    <t>Епік (приклад): Дизайн персонажів. Завдання (приклад): Розробити дизайн персонажів гри. Завдання (приклад): Створити анімації персонажів.</t>
-  </si>
-  <si>
-    <t>Епік (приклад): Координація заходу. Завдання (приклад): Координувати дії з виконавцями та артистами. Завдання (приклад): Організувати розклад заходу.</t>
-  </si>
-  <si>
-    <t>Епік (приклад): Робота зі ЗМІ. Завдання (приклад): Підготувати пресреліз для нового продукту. Завдання (приклад): Пропонувати історії журналістам.</t>
-  </si>
-  <si>
-    <t>Епік (приклад): Оцінка безпеки мережі. Завдання (приклад): Провести оцінку вразливостей. Завдання (приклад): Впровадити політики міжмережевого екрану.</t>
-  </si>
-  <si>
-    <t>Епік (приклад): Система зворотного зв'язку. Завдання (приклад): Розробити анкету для зворотного зв'язку від клієнтів. Завдання (приклад): Аналіз результатів опитування.</t>
-  </si>
-  <si>
-    <t>Епік (приклад): Управління посівами. Завдання (приклад): Планування сівозміни. Завдання (приклад): Моніторинг зростання врожаю.</t>
-  </si>
-  <si>
-    <t>Епік (приклад): Система управління трафіком. Завдання (приклад): Встановити розумні датчики трафіку. Завдання (приклад): Розробити алгоритми управління трафіком.</t>
-  </si>
-  <si>
-    <t>Приклади епіків та завдань</t>
   </si>
 </sst>
 </file>
@@ -628,10 +535,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D101"/>
+  <dimension ref="A1:C101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -639,11 +546,10 @@
     <col min="1" max="1" width="7.5546875" style="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="48.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="49" bestFit="1" customWidth="1"/>
-    <col min="5" max="26" width="8.6640625" customWidth="1"/>
+    <col min="4" max="25" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -653,11 +559,8 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -667,11 +570,8 @@
       <c r="C2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -681,11 +581,8 @@
       <c r="C3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -695,11 +592,8 @@
       <c r="C4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -709,11 +603,8 @@
       <c r="C5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -723,11 +614,8 @@
       <c r="C6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -737,11 +625,8 @@
       <c r="C7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -751,11 +636,8 @@
       <c r="C8" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -765,11 +647,8 @@
       <c r="C9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -779,11 +658,8 @@
       <c r="C10" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -793,11 +669,8 @@
       <c r="C11" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <v>11</v>
       </c>
@@ -807,11 +680,8 @@
       <c r="C12" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -821,11 +691,8 @@
       <c r="C13" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -835,11 +702,8 @@
       <c r="C14" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -849,11 +713,8 @@
       <c r="C15" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
         <v>15</v>
       </c>
@@ -863,11 +724,8 @@
       <c r="C16" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D16" s="3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -877,11 +735,8 @@
       <c r="C17" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D17" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="5">
         <v>17</v>
       </c>
@@ -891,11 +746,8 @@
       <c r="C18" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D18" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="5">
         <v>18</v>
       </c>
@@ -905,11 +757,8 @@
       <c r="C19" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D19" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="5">
         <v>19</v>
       </c>
@@ -919,11 +768,8 @@
       <c r="C20" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D20" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A21" s="5">
         <v>20</v>
       </c>
@@ -933,11 +779,8 @@
       <c r="C21" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D21" s="3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="5">
         <v>21</v>
       </c>
@@ -947,11 +790,8 @@
       <c r="C22" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D22" s="3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="5">
         <v>22</v>
       </c>
@@ -961,11 +801,8 @@
       <c r="C23" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D23" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A24" s="5">
         <v>23</v>
       </c>
@@ -975,11 +812,8 @@
       <c r="C24" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D24" s="3" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="5">
         <v>24</v>
       </c>
@@ -989,11 +823,8 @@
       <c r="C25" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D25" s="3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="5">
         <v>25</v>
       </c>
@@ -1003,11 +834,8 @@
       <c r="C26" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D26" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="5">
         <v>26</v>
       </c>
@@ -1017,11 +845,8 @@
       <c r="C27" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D27" s="3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="5">
         <v>27</v>
       </c>
@@ -1031,11 +856,8 @@
       <c r="C28" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D28" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" s="5">
         <v>28</v>
       </c>
@@ -1045,11 +867,8 @@
       <c r="C29" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="D29" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" s="5">
         <v>29</v>
       </c>
@@ -1059,11 +878,8 @@
       <c r="C30" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="D30" s="3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A31" s="5">
         <v>30</v>
       </c>
@@ -1073,11 +889,8 @@
       <c r="C31" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="D31" s="3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="6"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>

</xml_diff>